<commit_message>
Worked on sprint backlog, needs a bit more info. Will probably complete tomorrow
</commit_message>
<xml_diff>
--- a/Blackbear-Consultants_Deliverable_1_SprintBacklog_1.xlsx
+++ b/Blackbear-Consultants_Deliverable_1_SprintBacklog_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan\Desktop\College_Work\COS420\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skyzo\Desktop\College_Work\Blackbear-Consultants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4CA8A68-D376-437D-AE7F-A2C6D926B705}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CF93BD-30C4-4904-B429-35EB5A73AA22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{29D05152-AD15-448E-8A0D-C19F810C4EB6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{29D05152-AD15-448E-8A0D-C19F810C4EB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
   <si>
     <t>Sprint Goal</t>
   </si>
@@ -61,41 +61,71 @@
     <t>NF (Non-Functional)</t>
   </si>
   <si>
-    <t>Ethan Contribution</t>
-  </si>
-  <si>
-    <t>Abdullah Contribution</t>
-  </si>
-  <si>
-    <t>Jeremy Contribution</t>
-  </si>
-  <si>
-    <t>Mark Contribution</t>
-  </si>
-  <si>
-    <t>James Contribution</t>
-  </si>
-  <si>
-    <t>Chad Contribution</t>
-  </si>
-  <si>
-    <t>Ben Contribution</t>
-  </si>
-  <si>
-    <t>Begin application development and deliverable 1 documents</t>
-  </si>
-  <si>
     <t>Story</t>
   </si>
   <si>
     <t>KA (Knowledge Acquisition)</t>
+  </si>
+  <si>
+    <t>Complete mockup, user stories, and presentation to lay groundwork for writing code. Complete documentation for deliverable 1.</t>
+  </si>
+  <si>
+    <t>As a user (child), I want the game to seem fun and colorful so that I keep playing to learn my shapes and colors, while not seeming overly frustrating while learning.</t>
+  </si>
+  <si>
+    <t>As a user (parent), I want to be aware of what my child is working on so that I can positively reinforce them while at home.</t>
+  </si>
+  <si>
+    <t>As a user (instructor), I want the game to be locked in when I hand it to the child, so they cannot access any settings or sensitive information in the app</t>
+  </si>
+  <si>
+    <t>As a user (parent), I need the ability to continue teaching my children what they learned in school without the use of real world objects, because real world objects are expensive.</t>
+  </si>
+  <si>
+    <t>As a user (parent), I need an app that can help me automate the learning process of shapes and colors to reach more students.</t>
+  </si>
+  <si>
+    <t>As a user (parent), I want my child to learn shapes so that they easily recognize and understand shapes.</t>
+  </si>
+  <si>
+    <t>As a user (instructor), I want the interface of Teaching Tasks to be suitable for all of my clients (children) so that they will be able to properly use and learn from Teaching Tasks.</t>
+  </si>
+  <si>
+    <t>AK Contr.</t>
+  </si>
+  <si>
+    <t>EL Contr.</t>
+  </si>
+  <si>
+    <t>JH Contr.</t>
+  </si>
+  <si>
+    <t>MS Contr.</t>
+  </si>
+  <si>
+    <t>JW Contr.</t>
+  </si>
+  <si>
+    <t>BC Contr.</t>
+  </si>
+  <si>
+    <t>CB Contr.</t>
+  </si>
+  <si>
+    <t>NF (KA)</t>
+  </si>
+  <si>
+    <t>F (T)</t>
+  </si>
+  <si>
+    <t>F (KA)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,16 +148,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -200,12 +244,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
@@ -221,6 +276,29 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -539,108 +617,277 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBC36FCF-9F37-4AC5-B7F3-1DC0EDBEC864}">
   <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M11" sqref="M11:N15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="56.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" customWidth="1"/>
-    <col min="13" max="13" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="19" width="9.28515625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="59.88671875" customWidth="1"/>
+    <col min="2" max="2" width="95.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" customWidth="1"/>
+    <col min="13" max="13" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="19" width="9.33203125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:18" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="27.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="10">
+        <v>1</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="G2" s="10"/>
+      <c r="H2" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="I2" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+    </row>
+    <row r="3" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="18"/>
+      <c r="B3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="10">
+        <v>1</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+    </row>
+    <row r="4" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="18"/>
+      <c r="B4" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="10">
+        <v>1</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+    </row>
+    <row r="5" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="18"/>
+      <c r="B5" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="10">
+        <v>1</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+    </row>
+    <row r="6" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="18"/>
+      <c r="B6" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="10">
+        <v>1</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="18"/>
+      <c r="B7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C7" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="10">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+    </row>
+    <row r="8" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="18"/>
+      <c r="B8" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="10">
+        <v>1</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="M8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N8" s="5"/>
       <c r="Q8" s="8"/>
       <c r="R8" s="9"/>
     </row>
-    <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="M11" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="N11" s="5"/>
-    </row>
-    <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="M12" s="2" t="s">
+    <row r="9" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="M9" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="N12" s="3" t="s">
+      <c r="N9" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="M13" s="1" t="s">
+    <row r="10" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="M10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N13" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="M14" s="1" t="s">
+    <row r="11" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="M11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N14" s="1" t="s">
+      <c r="N11" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+    </row>
+    <row r="14" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+    </row>
+    <row r="15" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="M15" s="2"/>
-      <c r="N15" s="6" t="s">
-        <v>18</v>
-      </c>
+      <c r="N15" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -652,69 +899,111 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E3A477-5022-4EBF-A5F0-EFD4BBDA3FE6}">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.33203125" customWidth="1"/>
+    <col min="2" max="2" width="147.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8.77734375" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E1" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="F2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="18"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="18"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="18"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="18"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="18"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="18"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
       <c r="M8" s="4" t="s">
         <v>2</v>
       </c>
       <c r="N8" s="5"/>
     </row>
-    <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="M9" s="6" t="s">
         <v>3</v>
       </c>
@@ -722,7 +1011,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="M10" s="1" t="s">
         <v>7</v>
       </c>
@@ -730,7 +1019,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="M11" s="1" t="s">
         <v>8</v>
       </c>
@@ -738,13 +1027,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="M12" s="6"/>
       <c r="N12" s="6" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sprint backlog completed - still need to update contribution percentages
</commit_message>
<xml_diff>
--- a/Blackbear-Consultants_Deliverable_1_SprintBacklog_1.xlsx
+++ b/Blackbear-Consultants_Deliverable_1_SprintBacklog_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skyzo\Desktop\College_Work\Blackbear-Consultants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CF93BD-30C4-4904-B429-35EB5A73AA22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3081FBE7-C9C5-48F9-9B70-CEEF8EBC54E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{29D05152-AD15-448E-8A0D-C19F810C4EB6}"/>
   </bookViews>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
   <si>
     <t>Sprint Goal</t>
   </si>
@@ -260,7 +262,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
@@ -299,6 +301,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -617,7 +622,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBC36FCF-9F37-4AC5-B7F3-1DC0EDBEC864}">
   <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -641,8 +648,9 @@
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>9</v>
+      <c r="B1" s="14">
+        <f>+B12</f>
+        <v>0</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>3</v>
@@ -685,19 +693,27 @@
       <c r="D2" s="10">
         <v>1</v>
       </c>
-      <c r="E2" s="10"/>
+      <c r="E2" s="11">
+        <v>0</v>
+      </c>
       <c r="F2" s="11">
         <v>0.1</v>
       </c>
-      <c r="G2" s="10"/>
+      <c r="G2" s="11">
+        <v>0</v>
+      </c>
       <c r="H2" s="11">
         <v>0.1</v>
       </c>
       <c r="I2" s="11">
         <v>0.8</v>
       </c>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
+      <c r="J2" s="11">
+        <v>0</v>
+      </c>
+      <c r="K2" s="11">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="18"/>
@@ -710,13 +726,27 @@
       <c r="D3" s="10">
         <v>1</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
+      <c r="E3" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="F3" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="G3" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="H3" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="I3" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="J3" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="K3" s="19">
+        <v>0.14299999999999999</v>
+      </c>
     </row>
     <row r="4" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="18"/>
@@ -729,13 +759,27 @@
       <c r="D4" s="10">
         <v>1</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
+      <c r="E4" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="F4" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="G4" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="H4" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="I4" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="J4" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="K4" s="19">
+        <v>0.14299999999999999</v>
+      </c>
     </row>
     <row r="5" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="18"/>
@@ -748,13 +792,27 @@
       <c r="D5" s="10">
         <v>1</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
+      <c r="E5" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="F5" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="G5" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="H5" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="I5" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="J5" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="K5" s="19">
+        <v>0.14299999999999999</v>
+      </c>
     </row>
     <row r="6" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="18"/>
@@ -767,13 +825,27 @@
       <c r="D6" s="10">
         <v>1</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
+      <c r="E6" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="F6" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="G6" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="H6" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="I6" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="J6" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="K6" s="19">
+        <v>0.14299999999999999</v>
+      </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="18"/>
@@ -786,13 +858,27 @@
       <c r="D7" s="10">
         <v>1</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
+      <c r="E7" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="F7" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="G7" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="H7" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="I7" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="J7" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="K7" s="19">
+        <v>0.14299999999999999</v>
+      </c>
     </row>
     <row r="8" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="18"/>
@@ -805,13 +891,27 @@
       <c r="D8" s="10">
         <v>1</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
+      <c r="E8" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="F8" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="G8" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="H8" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="I8" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="J8" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="K8" s="19">
+        <v>0.14299999999999999</v>
+      </c>
       <c r="M8" s="4" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Update sprint backlog to accurately portray sprint events
</commit_message>
<xml_diff>
--- a/Blackbear-Consultants_Deliverable_1_SprintBacklog_1.xlsx
+++ b/Blackbear-Consultants_Deliverable_1_SprintBacklog_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skyzo\Desktop\College_Work\Blackbear-Consultants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3081FBE7-C9C5-48F9-9B70-CEEF8EBC54E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073D78D7-1633-488D-8FCD-40CAF331DBA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{29D05152-AD15-448E-8A0D-C19F810C4EB6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
   <si>
     <t>Sprint Goal</t>
   </si>
@@ -75,24 +75,6 @@
     <t>As a user (child), I want the game to seem fun and colorful so that I keep playing to learn my shapes and colors, while not seeming overly frustrating while learning.</t>
   </si>
   <si>
-    <t>As a user (parent), I want to be aware of what my child is working on so that I can positively reinforce them while at home.</t>
-  </si>
-  <si>
-    <t>As a user (instructor), I want the game to be locked in when I hand it to the child, so they cannot access any settings or sensitive information in the app</t>
-  </si>
-  <si>
-    <t>As a user (parent), I need the ability to continue teaching my children what they learned in school without the use of real world objects, because real world objects are expensive.</t>
-  </si>
-  <si>
-    <t>As a user (parent), I need an app that can help me automate the learning process of shapes and colors to reach more students.</t>
-  </si>
-  <si>
-    <t>As a user (parent), I want my child to learn shapes so that they easily recognize and understand shapes.</t>
-  </si>
-  <si>
-    <t>As a user (instructor), I want the interface of Teaching Tasks to be suitable for all of my clients (children) so that they will be able to properly use and learn from Teaching Tasks.</t>
-  </si>
-  <si>
     <t>AK Contr.</t>
   </si>
   <si>
@@ -114,13 +96,7 @@
     <t>CB Contr.</t>
   </si>
   <si>
-    <t>NF (KA)</t>
-  </si>
-  <si>
     <t>F (T)</t>
-  </si>
-  <si>
-    <t>F (KA)</t>
   </si>
 </sst>
 </file>
@@ -262,7 +238,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
@@ -303,6 +279,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -623,7 +608,7 @@
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -645,39 +630,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14">
-        <f>+B12</f>
-        <v>0</v>
+      <c r="B1" s="21" t="s">
+        <v>9</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="16" t="s">
+      <c r="E1" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="27.15" customHeight="1" x14ac:dyDescent="0.3">
@@ -688,7 +672,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D2" s="10">
         <v>1</v>
@@ -715,203 +699,77 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="18"/>
-      <c r="B3" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="10">
-        <v>1</v>
-      </c>
-      <c r="E3" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="F3" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="G3" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="H3" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="I3" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="J3" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="K3" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B3" s="12"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="18"/>
-      <c r="B4" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="10">
-        <v>1</v>
-      </c>
-      <c r="E4" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="F4" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="G4" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="H4" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="I4" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="J4" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="K4" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="12"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="18"/>
-      <c r="B5" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="10">
-        <v>1</v>
-      </c>
-      <c r="E5" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="F5" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="G5" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="H5" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="I5" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="J5" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="K5" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B5" s="12"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="18"/>
-      <c r="B6" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="10">
-        <v>1</v>
-      </c>
-      <c r="E6" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="F6" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="G6" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="H6" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="I6" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="J6" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="K6" s="19">
-        <v>0.14299999999999999</v>
-      </c>
+      <c r="B6" s="12"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="18"/>
-      <c r="B7" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="10">
-        <v>1</v>
-      </c>
-      <c r="E7" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="F7" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="G7" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="H7" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="I7" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="J7" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="K7" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B7" s="12"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+    </row>
+    <row r="8" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="18"/>
-      <c r="B8" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="10">
-        <v>1</v>
-      </c>
-      <c r="E8" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="F8" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="G8" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="H8" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="I8" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="J8" s="19">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="K8" s="19">
-        <v>0.14299999999999999</v>
-      </c>
+      <c r="B8" s="12"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
       <c r="M8" s="4" t="s">
         <v>2</v>
       </c>
@@ -1033,25 +891,25 @@
         <v>1</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F1" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="13" t="s">
         <v>19</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>